<commit_message>
Added RMA Test Cases: SO To inspection order SO to RMA Receipt
</commit_message>
<xml_diff>
--- a/templates/QA-Automation/Create Engineering Item Master.xlsx
+++ b/templates/QA-Automation/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="133">
   <si>
     <t>Item Number</t>
   </si>
@@ -433,6 +433,12 @@
   </si>
   <si>
     <t>a345f000000u4BJAAY</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-LQRXE</t>
+  </si>
+  <si>
+    <t>a345f000000u5GYAAY</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,6 +550,18 @@
       <color indexed="10"/>
       <b val="true"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -553,7 +571,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -579,11 +597,14 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -599,8 +620,10 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="11" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="13" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="15" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="7" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1035,9 +1058,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.70703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.6171875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.67578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.58203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.14453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1059,13 +1082,13 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misc Change-CPQ CRUD operations
</commit_message>
<xml_diff>
--- a/templates/QA-Automation/Create Engineering Item Master.xlsx
+++ b/templates/QA-Automation/Create Engineering Item Master.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\QA-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{B475F076-32FD-4CA1-963B-854C93D40CC5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B3836-406B-45C2-B879-96E99FB8E59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Create Engg Item" r:id="rId1" sheetId="1"/>
-    <sheet name="Routing Master" r:id="rId2" sheetId="2"/>
-    <sheet name="Operations" r:id="rId3" sheetId="3"/>
-    <sheet name="Add BOM" r:id="rId4" sheetId="4"/>
-    <sheet name="Create WO" r:id="rId5" sheetId="5"/>
-    <sheet name="Time and Qty Booking" r:id="rId6" sheetId="6"/>
-    <sheet name="WO receipt" r:id="rId7" sheetId="7"/>
+    <sheet name="Create Engg Item" sheetId="1" r:id="rId1"/>
+    <sheet name="Routing Master" sheetId="2" r:id="rId2"/>
+    <sheet name="Operations" sheetId="3" r:id="rId3"/>
+    <sheet name="Add BOM" sheetId="4" r:id="rId4"/>
+    <sheet name="Create WO" sheetId="5" r:id="rId5"/>
+    <sheet name="Time and Qty Booking" sheetId="6" r:id="rId6"/>
+    <sheet name="WO receipt" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="118">
   <si>
     <t>Item Number</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Add Inventory Item in Multiple Divisions Flag</t>
   </si>
   <si>
-    <t>Colorado (100)</t>
-  </si>
-  <si>
     <t>ProMake (No Track)</t>
   </si>
   <si>
@@ -393,63 +390,20 @@
     <t>Mayur Suryawanshi</t>
   </si>
   <si>
-    <t>Pro-PEItem-VZQHD</t>
-  </si>
-  <si>
-    <t>a345f000000u18KAAQ</t>
-  </si>
-  <si>
-    <t>Pro-PEItem-WL1AC</t>
-  </si>
-  <si>
-    <t>a345f000000u18PAAQ</t>
-  </si>
-  <si>
-    <t>Pro-PEItem-69XE7</t>
-  </si>
-  <si>
-    <t>a345f000000u1P0AAI</t>
-  </si>
-  <si>
-    <t>Pro-PEItem-KHNYD</t>
-  </si>
-  <si>
-    <t>a345f000000u1WMAAY</t>
-  </si>
-  <si>
-    <t>Pro-PEItem-IAJYN</t>
-  </si>
-  <si>
-    <t>a345f000000u2joAAA</t>
-  </si>
-  <si>
-    <t>Pro-PEItem-LQ1CH</t>
-  </si>
-  <si>
-    <t>a345f000000u4BEAAY</t>
-  </si>
-  <si>
-    <t>Pro-PEItem-QTLSN</t>
-  </si>
-  <si>
-    <t>a345f000000u4BJAAY</t>
-  </si>
-  <si>
-    <t>Pro-PEItem-LQRXE</t>
-  </si>
-  <si>
-    <t>a345f000000u5GYAAY</t>
+    <t>a345f000000uFjXAAU</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-H58GD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,90 +432,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -571,7 +441,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -579,57 +449,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="9" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="11" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="13" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="15" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="7" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -646,10 +481,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -684,7 +519,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -719,7 +554,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -813,21 +648,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -844,7 +679,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -896,40 +731,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.21875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="37.44140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="37.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -940,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -955,7 +790,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -990,37 +825,37 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
       <c r="K2" t="b">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
@@ -1029,10 +864,10 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="b">
         <v>0</v>
@@ -1042,30 +877,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFD7978-B775-4BD4-AD02-05C56EC9573E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFD7978-B775-4BD4-AD02-05C56EC9573E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.6171875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.67578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.14453125" collapsed="true"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1074,212 +909,212 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4468CCED-9303-4942-85BA-04C540AF4ED4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4468CCED-9303-4942-85BA-04C540AF4ED4}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.21875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="20.109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.21875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.21875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" t="s">
         <v>52</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>56</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>57</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>58</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>59</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2" t="s">
         <v>60</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>59</v>
-      </c>
-      <c r="R2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
-        <v>58</v>
-      </c>
-      <c r="V2" t="s">
-        <v>61</v>
-      </c>
-      <c r="W2" t="s">
-        <v>60</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -1291,49 +1126,49 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" t="s">
         <v>62</v>
       </c>
-      <c r="I3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
         <v>57</v>
       </c>
-      <c r="K3" t="s">
+      <c r="Q3" t="s">
         <v>58</v>
       </c>
-      <c r="L3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>59</v>
-      </c>
       <c r="R3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -1342,13 +1177,13 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X3">
         <v>1</v>
@@ -1360,65 +1195,65 @@
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
         <v>56</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>57</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>58</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>59</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" t="s">
         <v>60</v>
       </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="W4" t="s">
         <v>59</v>
       </c>
-      <c r="R4" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" t="s">
-        <v>61</v>
-      </c>
-      <c r="W4" t="s">
-        <v>60</v>
-      </c>
       <c r="X4">
         <v>1</v>
       </c>
@@ -1427,26 +1262,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F360E4A-BCCC-4DA8-B7DF-8940BA01DD94}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F360E4A-BCCC-4DA8-B7DF-8940BA01DD94}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.44140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1454,25 +1289,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1487,10 +1322,10 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1505,10 +1340,10 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1521,13 +1356,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00498F2-CC9D-4D63-B632-9B7CC73726CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00498F2-CC9D-4D63-B632-9B7CC73726CB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1536,66 +1371,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.88671875" collapsed="true"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="C2" s="1">
         <v>5</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
         <v>76</v>
       </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5329BA1-AB63-4C6D-BB5A-232013D72161}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5329BA1-AB63-4C6D-BB5A-232013D72161}">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1604,20 +1439,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="4.33203125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1625,58 +1460,58 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>82</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>84</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>85</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>86</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>87</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>88</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>89</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>90</v>
-      </c>
-      <c r="O1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="4">
         <v>44537</v>
@@ -1685,37 +1520,37 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" t="s">
         <v>93</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>94</v>
-      </c>
-      <c r="O2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -1724,25 +1559,25 @@
         <v>3</v>
       </c>
       <c r="N3" t="s">
+        <v>93</v>
+      </c>
+      <c r="O3" t="s">
         <v>94</v>
-      </c>
-      <c r="O3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -1751,19 +1586,19 @@
         <v>2</v>
       </c>
       <c r="N4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" t="s">
         <v>94</v>
       </c>
-      <c r="O4" t="s">
-        <v>95</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B55B6DD-20A8-4FAB-8155-791FB78D7E04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B55B6DD-20A8-4FAB-8155-791FB78D7E04}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1772,16 +1607,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.21875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1789,64 +1624,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
-      </c>
-      <c r="J1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>CONCATENATE('Routing Master'!B2," (",'Routing Master'!C2,")")</f>
-        <v>Pro-PEItem-VZQHD (Lot Track)</v>
+        <v>Pro-PEItem-H58GD (Lot Track)</v>
       </c>
       <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
         <v>106</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>107</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>108</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" t="s">
         <v>110</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>111</v>
       </c>
-      <c r="J2" t="s">
-        <v>112</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test cases for Recurring billing. Maintenance of other test cases
</commit_message>
<xml_diff>
--- a/templates/QA-Automation/Create Engineering Item Master.xlsx
+++ b/templates/QA-Automation/Create Engineering Item Master.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\QA-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B3836-406B-45C2-B879-96E99FB8E59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{892A1A25-FF5D-4D3A-98A1-2CB230C3CDA6}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Create Engg Item" sheetId="1" r:id="rId1"/>
-    <sheet name="Routing Master" sheetId="2" r:id="rId2"/>
-    <sheet name="Operations" sheetId="3" r:id="rId3"/>
-    <sheet name="Add BOM" sheetId="4" r:id="rId4"/>
-    <sheet name="Create WO" sheetId="5" r:id="rId5"/>
-    <sheet name="Time and Qty Booking" sheetId="6" r:id="rId6"/>
-    <sheet name="WO receipt" sheetId="7" r:id="rId7"/>
+    <sheet name="Create Engg Item" r:id="rId1" sheetId="1"/>
+    <sheet name="Routing Master" r:id="rId2" sheetId="2"/>
+    <sheet name="Operations" r:id="rId3" sheetId="3"/>
+    <sheet name="Add BOM" r:id="rId4" sheetId="4"/>
+    <sheet name="Create WO" r:id="rId5" sheetId="5"/>
+    <sheet name="Time and Qty Booking" r:id="rId6" sheetId="6"/>
+    <sheet name="WO receipt" r:id="rId7" sheetId="7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="125">
   <si>
     <t>Item Number</t>
   </si>
@@ -394,16 +394,38 @@
   </si>
   <si>
     <t>Pro-PEItem-H58GD</t>
+  </si>
+  <si>
+    <t>Colorado (100)</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-IPOKA</t>
+  </si>
+  <si>
+    <t>a345f000000uGVDAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-JHI3X</t>
+  </si>
+  <si>
+    <t>a345f000000uGVIAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-MFMOK</t>
+  </si>
+  <si>
+    <t>a345f000000uGVNAA2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +454,42 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -441,7 +499,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -449,22 +507,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="11">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -481,10 +554,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -519,7 +592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -554,7 +627,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -648,21 +721,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -679,7 +752,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -731,40 +804,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="37.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.21875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="37.44140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -828,7 +901,7 @@
         <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -877,13 +950,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFD7978-B775-4BD4-AD02-05C56EC9573E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFD7978-B775-4BD4-AD02-05C56EC9573E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -892,10 +965,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.171875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.66796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,23 +990,23 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
         <v>117</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4468CCED-9303-4942-85BA-04C540AF4ED4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4468CCED-9303-4942-85BA-04C540AF4ED4}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
@@ -942,33 +1015,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
@@ -1262,12 +1335,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F360E4A-BCCC-4DA8-B7DF-8940BA01DD94}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F360E4A-BCCC-4DA8-B7DF-8940BA01DD94}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1276,12 +1349,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1356,13 +1429,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00498F2-CC9D-4D63-B632-9B7CC73726CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00498F2-CC9D-4D63-B632-9B7CC73726CB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1371,12 +1444,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1425,12 +1498,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5329BA1-AB63-4C6D-BB5A-232013D72161}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5329BA1-AB63-4C6D-BB5A-232013D72161}">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1439,20 +1512,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="4.33203125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1593,12 +1666,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B55B6DD-20A8-4FAB-8155-791FB78D7E04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B55B6DD-20A8-4FAB-8155-791FB78D7E04}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1607,16 +1680,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.21875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1682,6 +1755,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>